<commit_message>
add logarithm piecewise McCormick
</commit_message>
<xml_diff>
--- a/examples/refinery_model/continous/refinery_continous.xlsx
+++ b/examples/refinery_model/continous/refinery_continous.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="700" windowWidth="33600" windowHeight="18720" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="38400" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DE" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="64">
   <si>
     <t>Size</t>
   </si>
@@ -629,6 +629,12 @@
       <t>/145.3
 7</t>
     </r>
+  </si>
+  <si>
+    <t>Bounds by piecewise McCormick n=10</t>
+  </si>
+  <si>
+    <t>Bounds by logarithm piecewise McCormick n=5</t>
   </si>
 </sst>
 </file>
@@ -1511,10 +1517,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D37" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2032,6 +2038,82 @@
         <v>7</v>
       </c>
     </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B34" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B35" s="3">
+        <v>5</v>
+      </c>
+      <c r="C35">
+        <v>-18380</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B36" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B37" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B38" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B39" s="3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B43" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B44" s="3">
+        <v>5</v>
+      </c>
+      <c r="C44">
+        <v>-18359</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B45" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B46" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B47" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B48" s="3">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2041,7 +2123,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update DE results for refinery
</commit_message>
<xml_diff>
--- a/examples/refinery_model/continous/refinery_continous.xlsx
+++ b/examples/refinery_model/continous/refinery_continous.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/canli/euler/.julia/v0.6/PlasmoAlgorithms/examples/refinery_model/continous/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/JuliaPro-0.6.4.1.app/Contents/Resources/pkgs-0.6.4.1/v0.6/PlasmoAlgorithms.jl/examples/refinery_model/continous/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2320" yWindow="1500" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="DE" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="66">
   <si>
     <t>Size</t>
   </si>
@@ -635,6 +635,12 @@
   </si>
   <si>
     <t>Bounds by logarithm piecewise McCormick n=5</t>
+  </si>
+  <si>
+    <t>no feasible point</t>
+  </si>
+  <si>
+    <t>&gt;10000</t>
   </si>
 </sst>
 </file>
@@ -780,7 +786,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -821,6 +827,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1108,8 +1117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="F27" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1204,6 +1213,9 @@
       <c r="G6" s="3">
         <v>120</v>
       </c>
+      <c r="H6" s="5">
+        <v>500</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
@@ -1224,6 +1236,9 @@
       <c r="G7" s="3">
         <v>-18041</v>
       </c>
+      <c r="H7">
+        <v>-17296</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
@@ -1244,13 +1259,16 @@
       <c r="G8" s="3">
         <v>-17888</v>
       </c>
+      <c r="H8">
+        <v>-17148.900000000001</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="4">
-        <f t="shared" ref="C9:G9" si="0">(C7-C8)/C7</f>
+        <f t="shared" ref="C9:H9" si="0">(C7-C8)/C7</f>
         <v>9.7996515679442506E-4</v>
       </c>
       <c r="D9" s="4">
@@ -1269,6 +1287,10 @@
         <f t="shared" si="0"/>
         <v>8.4806828889751121E-3</v>
       </c>
+      <c r="H9" s="4">
+        <f t="shared" si="0"/>
+        <v>8.5048566142459838E-3</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
@@ -1289,6 +1311,9 @@
       <c r="G10" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="H10" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -1314,6 +1339,9 @@
       <c r="G13" s="3">
         <v>120</v>
       </c>
+      <c r="H13" s="5">
+        <v>500</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
@@ -1334,6 +1362,9 @@
       <c r="G14" s="6">
         <v>-18042.25</v>
       </c>
+      <c r="H14" s="18">
+        <v>-17296</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
@@ -1354,6 +1385,9 @@
       <c r="G15" s="6">
         <v>-17888.13</v>
       </c>
+      <c r="H15" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
@@ -1379,8 +1413,11 @@
         <f>(G14-G15)/G14</f>
         <v>8.5421718466376969E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>13</v>
       </c>
@@ -1399,13 +1436,16 @@
       <c r="G17" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
         <v>9</v>
       </c>
@@ -1424,8 +1464,11 @@
       <c r="G20" s="3">
         <v>120</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H20" s="5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
         <v>10</v>
       </c>
@@ -1444,8 +1487,11 @@
       <c r="G21" s="6">
         <v>-17959.708574919499</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H21" s="20">
+        <v>-17297</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
         <v>11</v>
       </c>
@@ -1464,8 +1510,11 @@
       <c r="G22" s="6">
         <v>-17879.908697074901</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H22" s="18">
+        <v>-16369</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
         <v>12</v>
       </c>
@@ -1489,8 +1538,12 @@
         <f>(G21-G22)/G21</f>
         <v>4.4432724234756008E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H23" s="4">
+        <f t="shared" ref="H23" si="1">(H21-H22)/H21</f>
+        <v>5.3650922125224029E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
         <v>13</v>
       </c>
@@ -1507,6 +1560,9 @@
         <v>23</v>
       </c>
       <c r="G24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H24" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1519,8 +1575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1637,7 +1693,7 @@
         <v>-18503</v>
       </c>
       <c r="E5" s="4">
-        <f t="shared" ref="E5:E7" si="0">(D5-C5)/D5</f>
+        <f t="shared" ref="E5:E8" si="0">(D5-C5)/D5</f>
         <v>1.0376695670972274E-2</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -1714,6 +1770,24 @@
       </c>
       <c r="J7" s="5">
         <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="5">
+        <v>500</v>
+      </c>
+      <c r="C8">
+        <v>-17148</v>
+      </c>
+      <c r="D8">
+        <v>-17296</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" si="0"/>
+        <v>8.5568917668825163E-3</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add hull relaxation piecewise Mc for crude selection
</commit_message>
<xml_diff>
--- a/examples/refinery_model/continous/refinery_continous.xlsx
+++ b/examples/refinery_model/continous/refinery_continous.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/JuliaPro-0.6.4.1.app/Contents/Resources/pkgs-0.6.4.1/v0.6/PlasmoAlgorithms.jl/examples/refinery_model/continous/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/canli/euler/.julia/v0.6/PlasmoAlgorithms/examples/refinery_model/continous/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2320" yWindow="1500" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="41820" yWindow="880" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DE" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="70">
   <si>
     <t>Size</t>
   </si>
@@ -641,13 +641,25 @@
   </si>
   <si>
     <t>&gt;10000</t>
+  </si>
+  <si>
+    <t>Using convex hull of CNF</t>
+  </si>
+  <si>
+    <t>5 points</t>
+  </si>
+  <si>
+    <t>only solve one node</t>
+  </si>
+  <si>
+    <t>Using normal McCormick Envelope</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -702,6 +714,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -711,7 +730,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -774,6 +793,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -786,7 +842,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -830,6 +886,14 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1117,7 +1181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -1573,15 +1637,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
@@ -2187,6 +2252,336 @@
       <c r="B48" s="3">
         <v>120</v>
       </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B50" s="21"/>
+      <c r="C50" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="21"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="21"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="21"/>
+      <c r="B52" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F52" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G52" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H52" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I52" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="21"/>
+      <c r="B53" s="25">
+        <v>5</v>
+      </c>
+      <c r="C53" s="21">
+        <v>-18345</v>
+      </c>
+      <c r="D53" s="21">
+        <v>-18409</v>
+      </c>
+      <c r="E53" s="27">
+        <f>(D53-C53)/D53</f>
+        <v>3.4765603780759413E-3</v>
+      </c>
+      <c r="F53" s="21"/>
+      <c r="G53" s="21"/>
+      <c r="H53" s="21">
+        <v>317</v>
+      </c>
+      <c r="I53" s="21"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="21"/>
+      <c r="B54" s="25">
+        <v>10</v>
+      </c>
+      <c r="C54" s="23">
+        <v>-19427</v>
+      </c>
+      <c r="D54" s="23">
+        <v>-19474</v>
+      </c>
+      <c r="E54" s="27">
+        <f>(D54-C54)/D54</f>
+        <v>2.4134743760911986E-3</v>
+      </c>
+      <c r="F54" s="23"/>
+      <c r="G54" s="23"/>
+      <c r="H54" s="23">
+        <v>405</v>
+      </c>
+      <c r="I54" s="23"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="21"/>
+      <c r="B55" s="25">
+        <v>20</v>
+      </c>
+      <c r="C55" s="26">
+        <v>-18314</v>
+      </c>
+      <c r="D55" s="26">
+        <v>-18390</v>
+      </c>
+      <c r="E55" s="27">
+        <f>(D55-C55)/D55</f>
+        <v>4.1326808047852095E-3</v>
+      </c>
+      <c r="F55" s="26"/>
+      <c r="G55" s="26"/>
+      <c r="H55" s="26">
+        <v>389.1</v>
+      </c>
+      <c r="I55" s="26"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="21"/>
+      <c r="B56" s="25">
+        <v>40</v>
+      </c>
+      <c r="C56" s="26">
+        <v>-18337</v>
+      </c>
+      <c r="D56" s="26">
+        <v>-18499</v>
+      </c>
+      <c r="E56" s="27">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="F56" s="26"/>
+      <c r="G56" s="26"/>
+      <c r="H56" s="26">
+        <v>387</v>
+      </c>
+      <c r="I56" s="26"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="21"/>
+      <c r="B57" s="25">
+        <v>120</v>
+      </c>
+      <c r="C57" s="26">
+        <v>-17888</v>
+      </c>
+      <c r="D57" s="26">
+        <v>-17925</v>
+      </c>
+      <c r="E57" s="27">
+        <v>2.0999999999999999E-3</v>
+      </c>
+      <c r="F57" s="28"/>
+      <c r="G57" s="26"/>
+      <c r="H57" s="26">
+        <v>4027</v>
+      </c>
+      <c r="I57" s="26"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B63" s="21"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E63" s="21"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="21"/>
+      <c r="H63" s="21"/>
+      <c r="I63" s="21"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="21"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="21"/>
+      <c r="G64" s="21"/>
+      <c r="H64" s="21"/>
+      <c r="I64" s="21"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" s="21"/>
+      <c r="B65" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C65" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D65" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E65" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F65" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G65" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H65" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I65" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="21"/>
+      <c r="B66" s="25">
+        <v>5</v>
+      </c>
+      <c r="C66" s="21">
+        <v>-18276</v>
+      </c>
+      <c r="D66" s="21">
+        <v>-18696</v>
+      </c>
+      <c r="E66" s="27">
+        <f>(D66-C66)/D66</f>
+        <v>2.2464698331193838E-2</v>
+      </c>
+      <c r="F66" s="21"/>
+      <c r="G66" s="21"/>
+      <c r="H66" s="21">
+        <v>34</v>
+      </c>
+      <c r="I66" s="21"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" s="21"/>
+      <c r="B67" s="25">
+        <v>10</v>
+      </c>
+      <c r="C67" s="23">
+        <v>-19425</v>
+      </c>
+      <c r="D67" s="23">
+        <v>-19612</v>
+      </c>
+      <c r="E67" s="27">
+        <f>(D67-C67)/D67</f>
+        <v>9.5349785845400773E-3</v>
+      </c>
+      <c r="F67" s="23"/>
+      <c r="G67" s="23"/>
+      <c r="H67" s="23">
+        <v>47</v>
+      </c>
+      <c r="I67" s="23"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" s="21"/>
+      <c r="B68" s="25">
+        <v>20</v>
+      </c>
+      <c r="C68" s="26">
+        <v>-18313</v>
+      </c>
+      <c r="D68" s="26">
+        <v>-18523</v>
+      </c>
+      <c r="E68" s="27">
+        <f>(D68-C68)/D68</f>
+        <v>1.1337256383955083E-2</v>
+      </c>
+      <c r="F68" s="26"/>
+      <c r="G68" s="26"/>
+      <c r="H68" s="26">
+        <v>91</v>
+      </c>
+      <c r="I68" s="26"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" s="21"/>
+      <c r="B69" s="25">
+        <v>40</v>
+      </c>
+      <c r="C69" s="26">
+        <v>-18337</v>
+      </c>
+      <c r="D69" s="26">
+        <v>-18499</v>
+      </c>
+      <c r="E69" s="27">
+        <f>(D69-C69)/D69</f>
+        <v>8.7572301205470562E-3</v>
+      </c>
+      <c r="F69" s="26"/>
+      <c r="G69" s="26"/>
+      <c r="H69" s="26">
+        <v>184</v>
+      </c>
+      <c r="I69" s="26"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" s="21"/>
+      <c r="B70" s="25">
+        <v>120</v>
+      </c>
+      <c r="C70" s="26">
+        <v>-17887</v>
+      </c>
+      <c r="D70" s="26">
+        <v>-18043</v>
+      </c>
+      <c r="E70" s="27">
+        <f>(D70-C70)/D70</f>
+        <v>8.646012303940586E-3</v>
+      </c>
+      <c r="F70" s="28"/>
+      <c r="G70" s="26"/>
+      <c r="H70" s="26">
+        <v>473</v>
+      </c>
+      <c r="I70" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>